<commit_message>
add a default NA value for "duree/intensite/portee spatiale"
</commit_message>
<xml_diff>
--- a/app/model/ECOVAL.xlsx
+++ b/app/model/ECOVAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabricezaoui/Codes/ECOVAL/model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabricezaoui/Codes/ECOVAL/app/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEABC1A-EC42-764D-954C-381EAE470521}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303348F3-8C28-4F4E-9FBE-5D5C5B26213F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="741" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="741" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -1256,8 +1256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1335,7 +1335,7 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1343,7 +1343,7 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1351,7 +1351,7 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1702,7 +1702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
case "Diversité Espèce" -> "Diversité espèce"
</commit_message>
<xml_diff>
--- a/app/model/ECOVAL.xlsx
+++ b/app/model/ECOVAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabricezaoui/Codes/ECOVAL/app/model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabrice/Codes/ECOVAL/app/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303348F3-8C28-4F4E-9FBE-5D5C5B26213F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB591AB9-B7B2-4A49-9396-CA8C074E6272}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="741" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="741" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="186">
   <si>
     <t>Titre du projet</t>
   </si>
@@ -224,9 +224,6 @@
   </si>
   <si>
     <t>Longueur de lisière (Km) / surface de milieu forestier (Ha)</t>
-  </si>
-  <si>
-    <t>Diversité Espèce</t>
   </si>
   <si>
     <t>Diversité flore totale</t>
@@ -1005,246 +1002,246 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
         <v>48</v>
       </c>
       <c r="C1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" t="s">
         <v>116</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" t="s">
         <v>117</v>
       </c>
-      <c r="E1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>148</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>146</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>118</v>
-      </c>
-      <c r="I1" t="s">
-        <v>149</v>
-      </c>
-      <c r="J1" t="s">
-        <v>147</v>
-      </c>
-      <c r="K1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1256,7 +1253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1433,7 +1430,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -1441,7 +1438,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
@@ -1525,7 +1522,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
@@ -1533,7 +1530,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
@@ -1702,8 +1699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1734,27 +1731,27 @@
         <v>50</v>
       </c>
       <c r="E1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" t="s">
         <v>107</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>108</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>109</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>110</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>111</v>
-      </c>
-      <c r="J1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
         <v>51</v>
@@ -1768,7 +1765,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -1782,7 +1779,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -1796,7 +1793,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
         <v>51</v>
@@ -1810,7 +1807,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
         <v>51</v>
@@ -1824,7 +1821,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
         <v>51</v>
@@ -1838,7 +1835,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
         <v>51</v>
@@ -1852,7 +1849,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B9" t="s">
         <v>51</v>
@@ -1866,7 +1863,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B10" t="s">
         <v>51</v>
@@ -1880,7 +1877,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B11" t="s">
         <v>51</v>
@@ -1894,7 +1891,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B12" t="s">
         <v>51</v>
@@ -1908,7 +1905,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B13" t="s">
         <v>51</v>
@@ -1922,7 +1919,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B14" t="s">
         <v>51</v>
@@ -1936,13 +1933,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="C15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1950,13 +1947,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="C16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1964,13 +1961,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="C17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1978,13 +1975,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="C18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1992,13 +1989,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2006,13 +2003,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="C20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2020,13 +2017,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="C21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -2034,13 +2031,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="C22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -2048,13 +2045,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="C23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2062,13 +2059,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="C24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2076,13 +2073,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" t="s">
         <v>65</v>
-      </c>
-      <c r="C25" t="s">
-        <v>66</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -2090,13 +2087,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" t="s">
         <v>67</v>
-      </c>
-      <c r="C26" t="s">
-        <v>68</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -2104,13 +2101,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -2118,13 +2115,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2132,13 +2129,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2146,13 +2143,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -2160,13 +2157,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -2174,13 +2171,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -2188,13 +2185,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -2202,13 +2199,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -2216,13 +2213,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -2230,13 +2227,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -2244,13 +2241,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B37" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" t="s">
         <v>79</v>
-      </c>
-      <c r="C37" t="s">
-        <v>80</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -2258,13 +2255,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -2272,13 +2269,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -2286,13 +2283,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -2300,13 +2297,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -2314,13 +2311,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" t="s">
         <v>84</v>
-      </c>
-      <c r="C42" t="s">
-        <v>85</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -2328,13 +2325,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -2342,13 +2339,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -2356,13 +2353,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -2370,13 +2367,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -2384,13 +2381,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" t="s">
         <v>90</v>
-      </c>
-      <c r="C47" t="s">
-        <v>91</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -2398,13 +2395,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C48" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -2412,13 +2409,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C49" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -2426,13 +2423,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -2440,13 +2437,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B51" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" t="s">
         <v>95</v>
-      </c>
-      <c r="C51" t="s">
-        <v>96</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -2454,13 +2451,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -2468,13 +2465,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B53" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -2482,13 +2479,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C54" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -2496,13 +2493,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B55" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C55" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -2510,13 +2507,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -2524,13 +2521,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2538,13 +2535,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B58" t="s">
+        <v>101</v>
+      </c>
+      <c r="C58" t="s">
         <v>102</v>
-      </c>
-      <c r="C58" t="s">
-        <v>103</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -2552,13 +2549,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B59" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C59" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -2566,13 +2563,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C60" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -2580,13 +2577,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B61" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C61" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2594,13 +2591,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B62" t="s">
+        <v>104</v>
+      </c>
+      <c r="C62" t="s">
         <v>105</v>
-      </c>
-      <c r="C62" t="s">
-        <v>106</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -2635,323 +2632,323 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
         <v>48</v>
       </c>
       <c r="C1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" t="s">
         <v>116</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" t="s">
         <v>117</v>
       </c>
-      <c r="E1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>148</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>146</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>118</v>
-      </c>
-      <c r="I1" t="s">
-        <v>149</v>
-      </c>
-      <c r="J1" t="s">
-        <v>147</v>
-      </c>
-      <c r="K1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" t="s">
         <v>120</v>
-      </c>
-      <c r="C3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C17" t="s">
         <v>134</v>
-      </c>
-      <c r="C17" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
typo model habitat line 19
</commit_message>
<xml_diff>
--- a/app/model/ECOVAL.xlsx
+++ b/app/model/ECOVAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabrice/Codes/ECOVAL/app/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB591AB9-B7B2-4A49-9396-CA8C074E6272}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDCA663-DB57-9545-B987-8C32FB1A2A6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="741" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="741" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -442,9 +442,6 @@
     <t>Hauteur de chaque strate</t>
   </si>
   <si>
-    <t>Proportion de sol dégradé</t>
-  </si>
-  <si>
     <t>Nombre d'espèces indicatrices de pression</t>
   </si>
   <si>
@@ -520,9 +517,6 @@
     <t>Nombre de familles</t>
   </si>
   <si>
-    <t> Surface de milieu ne générant pas de perturbation</t>
-  </si>
-  <si>
     <t>Nombre d’observations de l’espèce</t>
   </si>
   <si>
@@ -587,6 +581,12 @@
   </si>
   <si>
     <t>% Milieux cultivés</t>
+  </si>
+  <si>
+    <t>Proportion de sol non dégradé</t>
+  </si>
+  <si>
+    <t>Surface de milieu ne générant pas de perturbation</t>
   </si>
 </sst>
 </file>
@@ -981,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1014,22 +1014,22 @@
         <v>116</v>
       </c>
       <c r="E1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H1" t="s">
         <v>117</v>
       </c>
       <c r="I1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K1" t="s">
         <v>118</v>
@@ -1037,211 +1037,211 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
         <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B3" t="s">
         <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B4" t="s">
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
         <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
         <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B7" t="s">
         <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s">
         <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B9" t="s">
         <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B10" t="s">
         <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B11" t="s">
         <v>78</v>
       </c>
       <c r="C11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B12" t="s">
         <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B13" t="s">
         <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s">
         <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B15" t="s">
         <v>119</v>
       </c>
       <c r="C15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B16" t="s">
         <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B17" t="s">
         <v>94</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B18" t="s">
         <v>94</v>
       </c>
       <c r="C18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B19" t="s">
         <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s">
         <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1430,7 +1430,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -1438,7 +1438,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
@@ -1522,7 +1522,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
@@ -1530,7 +1530,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
@@ -1699,7 +1699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="B15" sqref="B15:B25"/>
     </sheetView>
   </sheetViews>
@@ -1751,7 +1751,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
         <v>51</v>
@@ -1765,7 +1765,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -1779,7 +1779,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -1793,7 +1793,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
         <v>51</v>
@@ -1807,7 +1807,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
         <v>51</v>
@@ -1821,7 +1821,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B7" t="s">
         <v>51</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s">
         <v>51</v>
@@ -1849,7 +1849,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B9" t="s">
         <v>51</v>
@@ -1863,7 +1863,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B10" t="s">
         <v>51</v>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B11" t="s">
         <v>51</v>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B12" t="s">
         <v>51</v>
@@ -1905,7 +1905,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B13" t="s">
         <v>51</v>
@@ -1919,7 +1919,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s">
         <v>51</v>
@@ -1933,13 +1933,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B15" t="s">
         <v>119</v>
       </c>
       <c r="C15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1947,13 +1947,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B16" t="s">
         <v>119</v>
       </c>
       <c r="C16" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1961,13 +1961,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B17" t="s">
         <v>119</v>
       </c>
       <c r="C17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1975,13 +1975,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B18" t="s">
         <v>119</v>
       </c>
       <c r="C18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1989,13 +1989,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B19" t="s">
         <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2003,13 +2003,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B20" t="s">
         <v>119</v>
       </c>
       <c r="C20" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2017,13 +2017,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B21" t="s">
         <v>119</v>
       </c>
       <c r="C21" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -2031,13 +2031,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B22" t="s">
         <v>119</v>
       </c>
       <c r="C22" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -2045,13 +2045,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B23" t="s">
         <v>119</v>
       </c>
       <c r="C23" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2059,13 +2059,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B24" t="s">
         <v>119</v>
       </c>
       <c r="C24" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2073,7 +2073,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B25" t="s">
         <v>119</v>
@@ -2087,7 +2087,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B26" t="s">
         <v>66</v>
@@ -2101,7 +2101,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B27" t="s">
         <v>66</v>
@@ -2115,7 +2115,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B28" t="s">
         <v>66</v>
@@ -2129,7 +2129,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B29" t="s">
         <v>66</v>
@@ -2143,7 +2143,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B30" t="s">
         <v>66</v>
@@ -2157,7 +2157,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B31" t="s">
         <v>66</v>
@@ -2171,7 +2171,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B32" t="s">
         <v>66</v>
@@ -2185,7 +2185,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B33" t="s">
         <v>66</v>
@@ -2199,7 +2199,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B34" t="s">
         <v>66</v>
@@ -2213,7 +2213,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B35" t="s">
         <v>66</v>
@@ -2227,7 +2227,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B36" t="s">
         <v>66</v>
@@ -2241,7 +2241,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B37" t="s">
         <v>78</v>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B38" t="s">
         <v>78</v>
@@ -2269,7 +2269,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B39" t="s">
         <v>78</v>
@@ -2283,7 +2283,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B40" t="s">
         <v>78</v>
@@ -2297,7 +2297,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B41" t="s">
         <v>78</v>
@@ -2311,7 +2311,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B42" t="s">
         <v>83</v>
@@ -2325,7 +2325,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B43" t="s">
         <v>83</v>
@@ -2339,7 +2339,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B44" t="s">
         <v>83</v>
@@ -2353,7 +2353,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B45" t="s">
         <v>83</v>
@@ -2367,7 +2367,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B46" t="s">
         <v>83</v>
@@ -2381,7 +2381,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B47" t="s">
         <v>89</v>
@@ -2395,7 +2395,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B48" t="s">
         <v>89</v>
@@ -2409,7 +2409,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B49" t="s">
         <v>89</v>
@@ -2423,7 +2423,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B50" t="s">
         <v>89</v>
@@ -2437,7 +2437,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B51" t="s">
         <v>94</v>
@@ -2451,7 +2451,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B52" t="s">
         <v>94</v>
@@ -2465,7 +2465,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B53" t="s">
         <v>94</v>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B54" t="s">
         <v>94</v>
@@ -2493,7 +2493,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B55" t="s">
         <v>94</v>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B56" t="s">
         <v>94</v>
@@ -2521,7 +2521,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B57" t="s">
         <v>101</v>
@@ -2535,7 +2535,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B58" t="s">
         <v>101</v>
@@ -2549,7 +2549,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B59" t="s">
         <v>101</v>
@@ -2563,13 +2563,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B60" t="s">
         <v>104</v>
       </c>
       <c r="C60" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -2577,13 +2577,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B61" t="s">
         <v>104</v>
       </c>
       <c r="C61" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2591,7 +2591,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B62" t="s">
         <v>104</v>
@@ -2613,7 +2613,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2644,22 +2644,22 @@
         <v>116</v>
       </c>
       <c r="E1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H1" t="s">
         <v>117</v>
       </c>
       <c r="I1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K1" t="s">
         <v>118</v>
@@ -2667,18 +2667,18 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
         <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B3" t="s">
         <v>119</v>
@@ -2689,7 +2689,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B4" t="s">
         <v>78</v>
@@ -2700,7 +2700,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
         <v>78</v>
@@ -2711,7 +2711,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
         <v>78</v>
@@ -2722,7 +2722,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B7" t="s">
         <v>78</v>
@@ -2733,7 +2733,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s">
         <v>78</v>
@@ -2744,7 +2744,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B9" t="s">
         <v>78</v>
@@ -2755,18 +2755,18 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B10" t="s">
         <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B11" t="s">
         <v>78</v>
@@ -2777,7 +2777,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B12" t="s">
         <v>78</v>
@@ -2788,7 +2788,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B13" t="s">
         <v>78</v>
@@ -2799,7 +2799,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s">
         <v>78</v>
@@ -2810,7 +2810,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B15" t="s">
         <v>78</v>
@@ -2821,7 +2821,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B16" t="s">
         <v>78</v>
@@ -2832,7 +2832,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B17" t="s">
         <v>133</v>
@@ -2843,7 +2843,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B18" t="s">
         <v>133</v>
@@ -2854,7 +2854,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B19" t="s">
         <v>133</v>
@@ -2865,90 +2865,90 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B20" t="s">
         <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>137</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B21" t="s">
         <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B22" t="s">
         <v>83</v>
       </c>
       <c r="C22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B23" t="s">
         <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B24" t="s">
         <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B25" t="s">
         <v>89</v>
       </c>
       <c r="C25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B26" t="s">
         <v>94</v>
       </c>
       <c r="C26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B27" t="s">
         <v>94</v>
       </c>
       <c r="C27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add the general perimeter value
</commit_message>
<xml_diff>
--- a/app/model/ECOVAL.xlsx
+++ b/app/model/ECOVAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabrice/Codes/ECOVAL/app/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDCA663-DB57-9545-B987-8C32FB1A2A6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7811EA-307F-1643-8A24-36C4B71C4A47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="741" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6640" yWindow="8640" windowWidth="28800" windowHeight="17540" tabRatio="741" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="187">
   <si>
     <t>Titre du projet</t>
   </si>
@@ -587,6 +587,9 @@
   </si>
   <si>
     <t>Surface de milieu ne générant pas de perturbation</t>
+  </si>
+  <si>
+    <t>Perimetre</t>
   </si>
 </sst>
 </file>
@@ -981,7 +984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -1251,10 +1254,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1356,6 +1359,14 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B13" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change full name 'oiseaux nichant...'
</commit_message>
<xml_diff>
--- a/app/model/ECOVAL.xlsx
+++ b/app/model/ECOVAL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabrice/Codes/ECOVAL/app/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF1F9C9-E7D1-2243-96AC-D07B79BB9EA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AECFB71-1B7D-014A-B36F-21DECF151964}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="741" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="741" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -265,9 +265,6 @@
     <t>Fonctionnalité</t>
   </si>
   <si>
-    <t>Proportion d'oiseaux nicheurs</t>
-  </si>
-  <si>
     <t>Proportion d'espèces (hors oiseaux) se reproduisant sur le site</t>
   </si>
   <si>
@@ -587,6 +584,9 @@
   </si>
   <si>
     <t>Perimetre</t>
+  </si>
+  <si>
+    <t>Proportion d'oiseaux nichant sur le site</t>
   </si>
 </sst>
 </file>
@@ -981,7 +981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -1002,246 +1002,246 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
         <v>47</v>
       </c>
       <c r="C1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" t="s">
         <v>114</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H1" t="s">
         <v>115</v>
       </c>
-      <c r="E1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>145</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>143</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>116</v>
-      </c>
-      <c r="I1" t="s">
-        <v>146</v>
-      </c>
-      <c r="J1" t="s">
-        <v>144</v>
-      </c>
-      <c r="K1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
         <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
         <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
         <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B6" t="s">
         <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B7" t="s">
         <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B8" t="s">
         <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B9" t="s">
         <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B10" t="s">
         <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B11" t="s">
         <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B12" t="s">
         <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s">
         <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1361,7 +1361,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -1438,7 +1438,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -1446,7 +1446,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
@@ -1530,7 +1530,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
@@ -1538,7 +1538,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
@@ -1704,7 +1704,7 @@
   <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B25"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1735,27 +1735,27 @@
         <v>49</v>
       </c>
       <c r="E1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" t="s">
         <v>105</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>106</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>107</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>108</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>109</v>
-      </c>
-      <c r="J1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
         <v>50</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
         <v>50</v>
@@ -1783,7 +1783,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
@@ -1797,7 +1797,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
         <v>50</v>
@@ -1811,7 +1811,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B6" t="s">
         <v>50</v>
@@ -1825,7 +1825,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B7" t="s">
         <v>50</v>
@@ -1839,7 +1839,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B8" t="s">
         <v>50</v>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B9" t="s">
         <v>50</v>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B10" t="s">
         <v>50</v>
@@ -1881,7 +1881,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B11" t="s">
         <v>50</v>
@@ -1895,7 +1895,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B12" t="s">
         <v>50</v>
@@ -1909,7 +1909,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s">
         <v>50</v>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B14" t="s">
         <v>50</v>
@@ -1937,13 +1937,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1951,13 +1951,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1965,13 +1965,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1979,13 +1979,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1993,13 +1993,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2007,13 +2007,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2021,13 +2021,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -2035,13 +2035,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -2049,13 +2049,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2063,13 +2063,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2077,10 +2077,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C25" t="s">
         <v>64</v>
@@ -2091,7 +2091,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B26" t="s">
         <v>65</v>
@@ -2105,7 +2105,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B27" t="s">
         <v>65</v>
@@ -2119,7 +2119,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B28" t="s">
         <v>65</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B29" t="s">
         <v>65</v>
@@ -2147,7 +2147,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B30" t="s">
         <v>65</v>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B31" t="s">
         <v>65</v>
@@ -2175,7 +2175,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B32" t="s">
         <v>65</v>
@@ -2189,7 +2189,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B33" t="s">
         <v>65</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B34" t="s">
         <v>65</v>
@@ -2217,7 +2217,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B35" t="s">
         <v>65</v>
@@ -2231,7 +2231,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B36" t="s">
         <v>65</v>
@@ -2245,13 +2245,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B37" t="s">
         <v>77</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>185</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -2259,13 +2259,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B38" t="s">
         <v>77</v>
       </c>
       <c r="C38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -2273,13 +2273,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B39" t="s">
         <v>77</v>
       </c>
       <c r="C39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -2287,13 +2287,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B40" t="s">
         <v>77</v>
       </c>
       <c r="C40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -2301,13 +2301,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B41" t="s">
         <v>77</v>
       </c>
       <c r="C41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -2315,13 +2315,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" t="s">
         <v>82</v>
-      </c>
-      <c r="C42" t="s">
-        <v>83</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -2329,13 +2329,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -2343,13 +2343,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -2357,13 +2357,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -2371,13 +2371,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -2385,13 +2385,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B47" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" t="s">
         <v>88</v>
-      </c>
-      <c r="C47" t="s">
-        <v>89</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -2399,13 +2399,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -2413,13 +2413,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -2427,13 +2427,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -2441,13 +2441,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B51" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" t="s">
         <v>93</v>
-      </c>
-      <c r="C51" t="s">
-        <v>94</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -2455,13 +2455,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -2469,13 +2469,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C53" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -2483,13 +2483,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -2497,13 +2497,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B55" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C55" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -2511,13 +2511,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C56" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -2525,13 +2525,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2539,13 +2539,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B58" t="s">
+        <v>99</v>
+      </c>
+      <c r="C58" t="s">
         <v>100</v>
-      </c>
-      <c r="C58" t="s">
-        <v>101</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -2553,13 +2553,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B59" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C59" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -2567,13 +2567,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B60" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C60" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -2581,13 +2581,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B61" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C61" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2595,13 +2595,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B62" t="s">
+        <v>102</v>
+      </c>
+      <c r="C62" t="s">
         <v>103</v>
-      </c>
-      <c r="C62" t="s">
-        <v>104</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -2616,7 +2616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -2636,323 +2636,323 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
         <v>47</v>
       </c>
       <c r="C1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" t="s">
         <v>114</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H1" t="s">
         <v>115</v>
       </c>
-      <c r="E1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>145</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>143</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>116</v>
-      </c>
-      <c r="I1" t="s">
-        <v>146</v>
-      </c>
-      <c r="J1" t="s">
-        <v>144</v>
-      </c>
-      <c r="K1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
         <v>118</v>
-      </c>
-      <c r="C3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
         <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B6" t="s">
         <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B7" t="s">
         <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B8" t="s">
         <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B9" t="s">
         <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B10" t="s">
         <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B11" t="s">
         <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B12" t="s">
         <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s">
         <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B14" t="s">
         <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B15" t="s">
         <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B16" t="s">
         <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" t="s">
         <v>132</v>
-      </c>
-      <c r="C17" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
'Communauté faunistique' treated apart
</commit_message>
<xml_diff>
--- a/app/model/ECOVAL.xlsx
+++ b/app/model/ECOVAL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabrice/Codes/ECOVAL/app/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AECFB71-1B7D-014A-B36F-21DECF151964}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5695CC-2B37-CA43-969A-14551687C454}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="741" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="741" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="187">
   <si>
     <t>Titre du projet</t>
   </si>
@@ -587,6 +587,9 @@
   </si>
   <si>
     <t>Proportion d'oiseaux nichant sur le site</t>
+  </si>
+  <si>
+    <t>Communaute faunistique</t>
   </si>
 </sst>
 </file>
@@ -981,7 +984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -1375,9 +1378,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1449,6 +1452,14 @@
         <v>170</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>